<commit_message>
Make title of columns in the Database.xlsx
</commit_message>
<xml_diff>
--- a/ConsumptionCalculator/bin/Debug/Database.xlsx
+++ b/ConsumptionCalculator/bin/Debug/Database.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48071F57-3ABE-41D7-9ABE-CBB0102911E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DB4396-63E8-49EE-AD43-CF03E9776A47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Processors" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Socket 1151</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>Nvidia2</t>
+  </si>
+  <si>
+    <t>Производитель</t>
+  </si>
+  <si>
+    <t>Модель</t>
+  </si>
+  <si>
+    <t>Энергопотребление</t>
+  </si>
+  <si>
+    <t>Сокет</t>
   </si>
 </sst>
 </file>
@@ -391,32 +403,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="17.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>60</v>
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -424,27 +437,27 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1">
-        <v>95</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -455,9 +468,23 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D5" s="1">
         <v>125</v>
       </c>
     </row>
@@ -469,40 +496,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754E8CB3-B222-4BB6-ABFE-E010FE9691FE}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1">
-        <v>90</v>
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Make 3 links in different shops
</commit_message>
<xml_diff>
--- a/ConsumptionCalculator/bin/Debug/Database.xlsx
+++ b/ConsumptionCalculator/bin/Debug/Database.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338D4509-F638-4DE1-B31C-1430F597C9CE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395CE4A0-BB95-4C12-8510-F818BEAAE293}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Процессоры" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="137">
   <si>
     <t>Socket 1151</t>
   </si>
@@ -396,9 +396,6 @@
     <t>Radeon RX Vega 64</t>
   </si>
   <si>
-    <t>Ссылка на блок питания</t>
-  </si>
-  <si>
     <t>Максимальная мощность, Вт</t>
   </si>
   <si>
@@ -427,6 +424,15 @@
   </si>
   <si>
     <t>https://www.dns-shop.ru/product/9fc21a5f743f3120/blok-pitania-thermaltake-bajkal-1500w-w0431re/</t>
+  </si>
+  <si>
+    <t>Магазин 1</t>
+  </si>
+  <si>
+    <t>Магазин 2</t>
+  </si>
+  <si>
+    <t>Магазин 3</t>
   </si>
 </sst>
 </file>
@@ -531,7 +537,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -811,7 +817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -835,7 +841,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1813,7 +1819,7 @@
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2319,87 +2325,97 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="104.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="2" width="110.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="111.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="111.42578125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>250</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>350</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>450</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>550</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>650</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>750</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1000</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1600</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>